<commit_message>
update change point analysis, add fledge dates plot
</commit_message>
<xml_diff>
--- a/020_data/2021_NJ_chicks.xlsx
+++ b/020_data/2021_NJ_chicks.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/Hanks-Research/2020_Kestrel_Plots/020_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A88C25A-E472-9344-96E2-58A2FF325D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39DB3C95-37B3-6945-B89B-219AE09401B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="920" yWindow="460" windowWidth="24620" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="79">
   <si>
     <t>NESTBOX_ID</t>
   </si>
@@ -291,6 +291,9 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>banding date</t>
   </si>
 </sst>
 </file>
@@ -674,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O110"/>
+  <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -695,7 +698,7 @@
     <col min="14" max="14" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="3" customFormat="1" ht="43.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="43.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
@@ -741,8 +744,11 @@
       <c r="O1" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="P1" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2021</v>
       </c>
@@ -777,8 +783,11 @@
         <f>IF(J2="x","m","")&amp;IF(K2="x","f","")</f>
         <v>f</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="1">
+        <v>44353</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -802,7 +811,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -826,7 +835,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -850,7 +859,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -885,8 +894,11 @@
         <f t="shared" si="0"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P6" s="1">
+        <v>44355</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2021</v>
       </c>
@@ -908,7 +920,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -930,7 +942,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -954,7 +966,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -978,7 +990,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -1010,8 +1022,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P11" s="1">
+        <v>44368</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -1030,7 +1045,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -1065,8 +1080,11 @@
         <f t="shared" si="0"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P13" s="1">
+        <v>44362</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -1088,7 +1106,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -1110,7 +1128,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -1132,7 +1150,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="17" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -1156,7 +1174,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2021</v>
       </c>
@@ -1191,8 +1209,11 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P18" s="1">
+        <v>44340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2021</v>
       </c>
@@ -1214,7 +1235,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2021</v>
       </c>
@@ -1236,7 +1257,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2021</v>
       </c>
@@ -1261,7 +1282,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2021</v>
       </c>
@@ -1293,8 +1314,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P22" s="1">
+        <v>44362</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2021</v>
       </c>
@@ -1316,7 +1340,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2021</v>
       </c>
@@ -1348,8 +1372,11 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P24" s="4">
+        <v>44368</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2021</v>
       </c>
@@ -1368,7 +1395,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2021</v>
       </c>
@@ -1387,7 +1414,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2021</v>
       </c>
@@ -1409,7 +1436,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2021</v>
       </c>
@@ -1444,8 +1471,11 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P28" s="1">
+        <v>44362</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2021</v>
       </c>
@@ -1467,7 +1497,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2021</v>
       </c>
@@ -1489,7 +1519,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2021</v>
       </c>
@@ -1511,7 +1541,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2021</v>
       </c>
@@ -1533,7 +1563,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2021</v>
       </c>
@@ -1568,8 +1598,11 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P33" s="1">
+        <v>44349</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2021</v>
       </c>
@@ -1592,7 +1625,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2021</v>
       </c>
@@ -1615,7 +1648,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2021</v>
       </c>
@@ -1638,7 +1671,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2021</v>
       </c>
@@ -1673,8 +1706,11 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="P37" s="1">
+        <v>44368</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2021</v>
       </c>
@@ -1709,8 +1745,11 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P38" s="1">
+        <v>44368</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2021</v>
       </c>
@@ -1732,7 +1771,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2021</v>
       </c>
@@ -1754,7 +1793,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="41" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2021</v>
       </c>
@@ -1789,8 +1828,11 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P41" s="1">
+        <v>44340</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2021</v>
       </c>
@@ -1813,7 +1855,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2021</v>
       </c>
@@ -1836,7 +1878,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2021</v>
       </c>
@@ -1859,7 +1901,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2021</v>
       </c>
@@ -1882,7 +1924,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="46" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2021</v>
       </c>
@@ -1917,8 +1959,11 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P46" s="1">
+        <v>44363</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2021</v>
       </c>
@@ -1937,7 +1982,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2021</v>
       </c>
@@ -1959,7 +2004,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2021</v>
       </c>
@@ -1981,7 +2026,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2021</v>
       </c>
@@ -2003,7 +2048,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="51" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2021</v>
       </c>
@@ -2038,8 +2083,11 @@
         <f t="shared" si="0"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P51" s="1">
+        <v>44353</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2021</v>
       </c>
@@ -2062,7 +2110,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2021</v>
       </c>
@@ -2085,7 +2133,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="54" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2021</v>
       </c>
@@ -2120,8 +2168,11 @@
         <f t="shared" si="0"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P54" s="1">
+        <v>44362</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2021</v>
       </c>
@@ -2144,7 +2195,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2021</v>
       </c>
@@ -2167,7 +2218,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2021</v>
       </c>
@@ -2190,7 +2241,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="58" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2021</v>
       </c>
@@ -2225,8 +2276,11 @@
         <f t="shared" si="0"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P58" s="1">
+        <v>44349</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2021</v>
       </c>
@@ -2249,7 +2303,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2021</v>
       </c>
@@ -2272,7 +2326,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2021</v>
       </c>
@@ -2295,7 +2349,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2021</v>
       </c>
@@ -2318,7 +2372,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="63" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2021</v>
       </c>
@@ -2353,8 +2407,11 @@
         <f t="shared" si="0"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P63" s="1">
+        <v>44393</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2021</v>
       </c>
@@ -2377,7 +2434,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2021</v>
       </c>
@@ -2397,7 +2454,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2021</v>
       </c>
@@ -2420,7 +2477,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2021</v>
       </c>
@@ -2455,8 +2512,11 @@
         <f t="shared" ref="O67:O101" si="1">IF(J67="x","m","")&amp;IF(K67="x","f","")</f>
         <v>f</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P67" s="1">
+        <v>44355</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2021</v>
       </c>
@@ -2478,7 +2538,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2021</v>
       </c>
@@ -2500,7 +2560,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2021</v>
       </c>
@@ -2522,7 +2582,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2021</v>
       </c>
@@ -2544,7 +2604,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="72" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2021</v>
       </c>
@@ -2579,8 +2639,11 @@
         <f t="shared" si="1"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P72" s="1">
+        <v>44349</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2021</v>
       </c>
@@ -2603,7 +2666,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2021</v>
       </c>
@@ -2623,7 +2686,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2021</v>
       </c>
@@ -2646,7 +2709,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="76" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2021</v>
       </c>
@@ -2670,7 +2733,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2021</v>
       </c>
@@ -2702,8 +2765,11 @@
         <f t="shared" si="1"/>
         <v/>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P77" s="1">
+        <v>44355</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2021</v>
       </c>
@@ -2725,7 +2791,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2021</v>
       </c>
@@ -2747,7 +2813,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2021</v>
       </c>
@@ -2769,7 +2835,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2021</v>
       </c>
@@ -2791,7 +2857,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="82" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2021</v>
       </c>
@@ -2826,8 +2892,11 @@
         <f t="shared" si="1"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P82" s="1">
+        <v>44353</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2021</v>
       </c>
@@ -2849,7 +2918,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2021</v>
       </c>
@@ -2871,7 +2940,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2021</v>
       </c>
@@ -2893,7 +2962,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2021</v>
       </c>
@@ -2915,7 +2984,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="87" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2021</v>
       </c>
@@ -2950,8 +3019,11 @@
         <f t="shared" si="1"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P87" s="1">
+        <v>44349</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2021</v>
       </c>
@@ -2974,7 +3046,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2021</v>
       </c>
@@ -2997,7 +3069,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2021</v>
       </c>
@@ -3020,7 +3092,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>2021</v>
       </c>
@@ -3043,7 +3115,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="92" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>2021</v>
       </c>
@@ -3067,7 +3139,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>2021</v>
       </c>
@@ -3102,8 +3174,11 @@
         <f t="shared" si="1"/>
         <v>f</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P93" s="1">
+        <v>44355</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>2021</v>
       </c>
@@ -3126,7 +3201,7 @@
         <v>f</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>2021</v>
       </c>
@@ -3149,7 +3224,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2021</v>
       </c>
@@ -3172,7 +3247,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2021</v>
       </c>
@@ -3192,7 +3267,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2021</v>
       </c>
@@ -3227,8 +3302,11 @@
         <f t="shared" si="1"/>
         <v>m</v>
       </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P98" s="1">
+        <v>44393</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2021</v>
       </c>
@@ -3246,7 +3324,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2021</v>
       </c>
@@ -3267,7 +3345,7 @@
         <v>m</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2021</v>
       </c>
@@ -3288,31 +3366,31 @@
         <v>m</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E102"/>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E103"/>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E104"/>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E105"/>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E106"/>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E107"/>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E108"/>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E109"/>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E110"/>
     </row>
   </sheetData>

</xml_diff>